<commit_message>
omg max just order
</commit_message>
<xml_diff>
--- a/MING_RTD_BOARD/Project Outputs for MING_RTD_BOARD/MING_RTD_BOARD BOM.xlsx
+++ b/MING_RTD_BOARD/Project Outputs for MING_RTD_BOARD/MING_RTD_BOARD BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mingw\Documents\GitHub\RTD-Breakout-Board\MING_RTD_BOARD\Project Outputs for MING_RTD_BOARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23EEDFF3-BD37-4F3F-8F10-8807566C33CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FB6C1AD-4AB4-4285-BC49-1FA8F47EBF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{5DBFCF24-DDB1-417C-A890-126D621F8A6F}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{F5B4F360-B6D4-4E86-A859-F7F409B3CE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="MING_RTD_BOARD BOM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Comment</t>
   </si>
@@ -67,13 +67,13 @@
     <t/>
   </si>
   <si>
-    <t>C1, C2, C3, C5, C6</t>
+    <t>C1, C2, C3, C5</t>
   </si>
   <si>
     <t>FP-GCM188-0_1-IPC_C</t>
   </si>
   <si>
-    <t>C83054</t>
+    <t>C307331</t>
   </si>
   <si>
     <t>30pF</t>
@@ -112,13 +112,16 @@
     <t>C20079</t>
   </si>
   <si>
-    <t>Blue LED</t>
+    <t>Blue LED 0603</t>
+  </si>
+  <si>
+    <t>Blue 465~475nm 0603 Light Emitting Diodes (LED) ROHS</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>C165977</t>
+    <t>C72041</t>
   </si>
   <si>
     <t>5k1</t>
@@ -175,6 +178,21 @@
     <t>C779509</t>
   </si>
   <si>
+    <t>C183880</t>
+  </si>
+  <si>
+    <t>6V - - - Fixed 3.3V SOT-23-3L Linear Voltage Regulators (LDO) ROHS</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>FP-SOT23-IPC_C</t>
+  </si>
+  <si>
+    <t>LN1121P332MR-G</t>
+  </si>
+  <si>
     <t>ATMEGA328P-AU</t>
   </si>
   <si>
@@ -188,21 +206,6 @@
   </si>
   <si>
     <t>C14877</t>
-  </si>
-  <si>
-    <t>C183880</t>
-  </si>
-  <si>
-    <t>6V - - - Fixed 3.3V SOT-23-3L Linear Voltage Regulators (LDO) ROHS</t>
-  </si>
-  <si>
-    <t>U?</t>
-  </si>
-  <si>
-    <t>FP-SOT23-IPC_C</t>
-  </si>
-  <si>
-    <t>LN1121P332MR-G</t>
   </si>
   <si>
     <t>8Mhz Oscillator</t>
@@ -590,7 +593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD5B498-3097-4756-B32F-0F6CBC6AB754}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF454343-0534-4E19-B40C-22FAD7DD6CF5}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -655,7 +658,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -720,15 +723,17 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -736,17 +741,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -754,17 +759,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -772,17 +777,17 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -790,17 +795,17 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -808,19 +813,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -828,19 +833,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -848,19 +853,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -868,19 +873,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>

</xml_diff>